<commit_message>
Identifies local and external references in formulae.
</commit_message>
<xml_diff>
--- a/Simplified forecaster.xlsx
+++ b/Simplified forecaster.xlsx
@@ -5,18 +5,23 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WoodwardS\Documents\Future Projects\NZAEL Spreadsheet\excel_crawler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WoodwardS\Documents\Future Projects\NZAEL Spreadsheet\excel2r\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24720" yWindow="0" windowWidth="25200" windowHeight="11235"/>
+    <workbookView xWindow="30900" yWindow="0" windowWidth="25200" windowHeight="11235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Some Inputs" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <definedNames>
     <definedName name="Assets">Sheet1!$D$4</definedName>
-    <definedName name="Ha">Sheet1!$D$3</definedName>
+    <definedName name="Ha">'Some Inputs'!$D$3</definedName>
     <definedName name="Test">#REF!</definedName>
     <definedName name="WorkingTable">Sheet1!$A$19:$M$35</definedName>
   </definedNames>
@@ -168,7 +173,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,6 +192,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -225,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -234,6 +246,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -736,7 +750,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D99B0BD9-FA83-44F5-B840-F18FCDB3C27F}</c15:txfldGUID>
+                      <c15:txfldGUID>{2E6AC211-0F0B-4077-97C0-EC52FB83B69B}</c15:txfldGUID>
                       <c15:f>Sheet1!$Q$21</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -777,7 +791,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{FC3EA6D5-2809-4B73-98AD-348A72B5DBF9}</c15:txfldGUID>
+                      <c15:txfldGUID>{0FA701F8-EF94-41ED-8BEF-EC8300165BB4}</c15:txfldGUID>
                       <c15:f>Sheet1!$Q$22</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -818,7 +832,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{BCD9D4B6-DB21-408C-9EF4-DA58A2BB66E2}</c15:txfldGUID>
+                      <c15:txfldGUID>{880687E2-99D3-4F4E-9643-5EA83C0B1E2F}</c15:txfldGUID>
                       <c15:f>Sheet1!$Q$23</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1655,15 +1669,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1683,6 +1697,48 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet 2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="G3">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Goob_ (1)"/>
+      <sheetName val="Sheet 2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="C4">
+            <v>4</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1984,8 +2040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2003,10 +2059,12 @@
       <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="9" t="str">
+        <f>'Some Inputs'!C3</f>
+        <v>Ha</v>
+      </c>
+      <c r="D3" s="9">
+        <f>'Some Inputs'!D3</f>
         <v>100</v>
       </c>
     </row>
@@ -2021,7 +2079,7 @@
         <v>6</v>
       </c>
       <c r="G4">
-        <f>+D4*D3</f>
+        <f>+D4*'Some Inputs'!D3</f>
         <v>5000000</v>
       </c>
     </row>
@@ -2075,7 +2133,7 @@
         <v>10</v>
       </c>
       <c r="G9">
-        <f>+D9*D3</f>
+        <f>+D9*'Some Inputs'!D3</f>
         <v>105000</v>
       </c>
     </row>
@@ -2267,8 +2325,8 @@
       <c r="B21" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="6">
-        <f>+$G$5</f>
+      <c r="C21" s="8">
+        <f>Sheet1!$G$5</f>
         <v>2500000</v>
       </c>
       <c r="D21">
@@ -2328,7 +2386,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="6">
-        <f t="shared" ref="C22:C23" si="3">+$G$5</f>
+        <f>Sheet1!$G$5</f>
         <v>2500000</v>
       </c>
       <c r="D22">
@@ -2336,43 +2394,43 @@
         <v>2562000</v>
       </c>
       <c r="E22">
-        <f t="shared" ref="E22:M22" si="4">+$G$4-D26+D34</f>
+        <f t="shared" ref="E22:M22" si="3">+$G$4-D26+D34</f>
         <v>2627410</v>
       </c>
       <c r="F22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2696417.5500000003</v>
       </c>
       <c r="G22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2769220.5152500002</v>
       </c>
       <c r="H22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2846027.6435887502</v>
       </c>
       <c r="I22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2927059.1639861315</v>
       </c>
       <c r="J22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3012547.4180053687</v>
       </c>
       <c r="K22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3102737.5259956638</v>
       </c>
       <c r="L22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3197888.0899254256</v>
       </c>
       <c r="M22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3298271.9348713239</v>
       </c>
       <c r="O22">
-        <f t="shared" ref="O22:O23" si="5">+$M$20</f>
+        <f t="shared" ref="O22:O23" si="4">+$M$20</f>
         <v>10</v>
       </c>
       <c r="P22">
@@ -2388,7 +2446,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="6">
-        <f t="shared" si="3"/>
+        <f>+$G$5</f>
         <v>2500000</v>
       </c>
       <c r="D23">
@@ -2396,43 +2454,43 @@
         <v>2509500</v>
       </c>
       <c r="E23">
-        <f t="shared" ref="E23:M23" si="6">+$G$4-D27+D35</f>
+        <f t="shared" ref="E23:M23" si="5">+$G$4-D27+D35</f>
         <v>2519522.5</v>
       </c>
       <c r="F23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2530096.2374999998</v>
       </c>
       <c r="G23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2541251.5305625</v>
       </c>
       <c r="H23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2553020.3647434376</v>
       </c>
       <c r="I23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2565436.4848043267</v>
       </c>
       <c r="J23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2578535.4914685646</v>
       </c>
       <c r="K23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2592354.9434993356</v>
       </c>
       <c r="L23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2606934.4653917989</v>
       </c>
       <c r="M23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2622315.8609883478</v>
       </c>
       <c r="O23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="P23">
@@ -2458,43 +2516,43 @@
         <v>2500000</v>
       </c>
       <c r="D25">
-        <f t="shared" ref="D25:M25" si="7">+$G$4-D21</f>
+        <f t="shared" ref="D25:M25" si="6">+$G$4-D21</f>
         <v>2385500</v>
       </c>
       <c r="E25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>2264702.5</v>
       </c>
       <c r="F25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>2137261.1374999997</v>
       </c>
       <c r="G25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>2002810.5000624997</v>
       </c>
       <c r="H25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1860965.0775659373</v>
       </c>
       <c r="I25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1711318.1568320636</v>
       </c>
       <c r="J25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1553440.6554578273</v>
       </c>
       <c r="K25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1386879.8915080079</v>
       </c>
       <c r="L25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1211158.2855409482</v>
       </c>
       <c r="M25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1025771.9912457</v>
       </c>
     </row>
@@ -2503,47 +2561,47 @@
         <v>18</v>
       </c>
       <c r="C26" s="6">
-        <f t="shared" ref="C26:M27" si="8">+$G$4-C22</f>
+        <f t="shared" ref="C26:M27" si="7">+$G$4-C22</f>
         <v>2500000</v>
       </c>
       <c r="D26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2438000</v>
       </c>
       <c r="E26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2372590</v>
       </c>
       <c r="F26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2303582.4499999997</v>
       </c>
       <c r="G26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2230779.4847499998</v>
       </c>
       <c r="H26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2153972.3564112498</v>
       </c>
       <c r="I26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2072940.8360138685</v>
       </c>
       <c r="J26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1987452.5819946313</v>
       </c>
       <c r="K26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1897262.4740043362</v>
       </c>
       <c r="L26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1802111.9100745744</v>
       </c>
       <c r="M26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1701728.0651286761</v>
       </c>
     </row>
@@ -2552,47 +2610,47 @@
         <v>19</v>
       </c>
       <c r="C27" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2500000</v>
       </c>
       <c r="D27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2490500</v>
       </c>
       <c r="E27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2480477.5</v>
       </c>
       <c r="F27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2469903.7625000002</v>
       </c>
       <c r="G27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2458748.4694375</v>
       </c>
       <c r="H27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2446979.6352565624</v>
       </c>
       <c r="I27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2434563.5151956733</v>
       </c>
       <c r="J27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2421464.5085314354</v>
       </c>
       <c r="K27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2407645.0565006644</v>
       </c>
       <c r="L27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2393065.5346082011</v>
       </c>
       <c r="M27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2377684.1390116522</v>
       </c>
     </row>
@@ -2611,43 +2669,43 @@
         <v>137500</v>
       </c>
       <c r="D29">
-        <f t="shared" ref="D29:M29" si="9">+D25*$D$6</f>
+        <f t="shared" ref="D29:M29" si="8">+D25*$D$6</f>
         <v>131202.5</v>
       </c>
       <c r="E29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>124558.6375</v>
       </c>
       <c r="F29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>117549.36256249998</v>
       </c>
       <c r="G29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>110154.57750343748</v>
       </c>
       <c r="H29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>102353.07926612656</v>
       </c>
       <c r="I29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>94122.498625763503</v>
       </c>
       <c r="J29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>85439.236050180494</v>
       </c>
       <c r="K29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>76278.394032940429</v>
       </c>
       <c r="L29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>66613.705704752152</v>
       </c>
       <c r="M29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>56417.459518513504</v>
       </c>
     </row>
@@ -2656,47 +2714,47 @@
         <v>18</v>
       </c>
       <c r="C30" s="6">
-        <f t="shared" ref="C30:M31" si="10">+C26*$D$6</f>
+        <f t="shared" ref="C30:M31" si="9">+C26*$D$6</f>
         <v>137500</v>
       </c>
       <c r="D30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>134090</v>
       </c>
       <c r="E30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>130492.45</v>
       </c>
       <c r="F30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>126697.03474999999</v>
       </c>
       <c r="G30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>122692.87166124998</v>
       </c>
       <c r="H30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>118468.47960261874</v>
       </c>
       <c r="I30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>114011.74598076276</v>
       </c>
       <c r="J30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>109309.89200970472</v>
       </c>
       <c r="K30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>104349.43607023849</v>
       </c>
       <c r="L30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>99116.155054101589</v>
       </c>
       <c r="M30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>93595.043582077182</v>
       </c>
     </row>
@@ -2705,47 +2763,47 @@
         <v>19</v>
       </c>
       <c r="C31" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>137500</v>
       </c>
       <c r="D31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>136977.5</v>
       </c>
       <c r="E31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>136426.26250000001</v>
       </c>
       <c r="F31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>135844.70693750001</v>
       </c>
       <c r="G31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>135231.1658190625</v>
       </c>
       <c r="H31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>134583.87993911092</v>
       </c>
       <c r="I31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>133900.99333576203</v>
       </c>
       <c r="J31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>133180.54796922894</v>
       </c>
       <c r="K31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>132420.47810753653</v>
       </c>
       <c r="L31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>131618.60440345106</v>
       </c>
       <c r="M31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>130772.62764564087</v>
       </c>
     </row>
@@ -2764,43 +2822,43 @@
         <v>114500.00000000006</v>
       </c>
       <c r="D33">
-        <f t="shared" ref="D33:M33" si="11">+$G$10-$G12-D29</f>
+        <f t="shared" ref="D33:M33" si="10">+$G$10-$G12-D29</f>
         <v>120797.50000000006</v>
       </c>
       <c r="E33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>127441.36250000006</v>
       </c>
       <c r="F33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>134450.63743750006</v>
       </c>
       <c r="G33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>141845.42249656259</v>
       </c>
       <c r="H33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>149646.9207338735</v>
       </c>
       <c r="I33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>157877.50137423654</v>
       </c>
       <c r="J33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>166560.76394981955</v>
       </c>
       <c r="K33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>175721.60596705962</v>
       </c>
       <c r="L33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>185386.29429524791</v>
       </c>
       <c r="M33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>195582.54048148656</v>
       </c>
     </row>
@@ -2809,47 +2867,47 @@
         <v>18</v>
       </c>
       <c r="C34" s="6">
-        <f t="shared" ref="C34:M35" si="12">+$G$10-$G13-C30</f>
+        <f t="shared" ref="C34:M35" si="11">+$G$10-$G13-C30</f>
         <v>62000.000000000058</v>
       </c>
       <c r="D34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>65410.000000000058</v>
       </c>
       <c r="E34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>69007.550000000061</v>
       </c>
       <c r="F34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>72802.965250000067</v>
       </c>
       <c r="G34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>76807.128338750073</v>
       </c>
       <c r="H34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>81031.520397381319</v>
       </c>
       <c r="I34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>85488.254019237298</v>
       </c>
       <c r="J34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>90190.107990295335</v>
       </c>
       <c r="K34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>95150.563929761571</v>
       </c>
       <c r="L34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>100383.84494589847</v>
       </c>
       <c r="M34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>105904.95641792288</v>
       </c>
     </row>
@@ -2858,47 +2916,47 @@
         <v>19</v>
       </c>
       <c r="C35" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>9500</v>
       </c>
       <c r="D35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>10022.5</v>
       </c>
       <c r="E35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>10573.737499999988</v>
       </c>
       <c r="F35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>11155.293062499986</v>
       </c>
       <c r="G35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>11768.834180937498</v>
       </c>
       <c r="H35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>12416.120060889079</v>
       </c>
       <c r="I35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>13099.006664237968</v>
       </c>
       <c r="J35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>13819.452030771063</v>
       </c>
       <c r="K35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>14579.521892463468</v>
       </c>
       <c r="L35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>15381.395596548944</v>
       </c>
       <c r="M35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>16227.372354359133</v>
       </c>
     </row>
@@ -2911,43 +2969,43 @@
         <v>62000.000000000036</v>
       </c>
       <c r="D37">
-        <f t="shared" ref="D37:M37" si="13">AVERAGE(D33:D35)</f>
+        <f t="shared" ref="D37:M37" si="12">AVERAGE(D33:D35)</f>
         <v>65410.000000000036</v>
       </c>
       <c r="E37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>69007.550000000032</v>
       </c>
       <c r="F37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>72802.965250000037</v>
       </c>
       <c r="G37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>76807.128338750059</v>
       </c>
       <c r="H37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>81031.520397381304</v>
       </c>
       <c r="I37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>85488.254019237269</v>
       </c>
       <c r="J37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>90190.107990295321</v>
       </c>
       <c r="K37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>95150.563929761571</v>
       </c>
       <c r="L37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>100383.84494589844</v>
       </c>
       <c r="M37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>105904.95641792286</v>
       </c>
     </row>
@@ -2956,4 +3014,57 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="str">
+        <f>Sheet1!C3</f>
+        <v>Ha</v>
+      </c>
+      <c r="D4">
+        <f>Sheet1!D3</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="str">
+        <f>Sheet1!C4</f>
+        <v>Assets/ha</v>
+      </c>
+      <c r="D5">
+        <f>[1]Sheet1!$G$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="str">
+        <f>Sheet1!C5</f>
+        <v>Debt:Assets</v>
+      </c>
+      <c r="D6">
+        <f>'[2]Goob_ (1)'!$C$4</f>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>